<commit_message>
Robot 15 and 16; mentions added back
</commit_message>
<xml_diff>
--- a/Robot15_GetTweetsBetweenTwoDates/Tweets.xlsx
+++ b/Robot15_GetTweetsBetweenTwoDates/Tweets.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UiPath Course\UiPathRobots\Robot15_GetTweetsBetweenTwoDates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahmutfikret.gezer\Documents\GitHub\UiPathRobots\Robot15_GetTweetsBetweenTwoDates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9B0F59B-FFF5-4010-AA35-C7261217CAB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAAC7A7D-9103-4A11-B8B5-D51E8A0F613D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{42AA605B-8E83-410B-8385-520117E1EEB3}"/>
+    <workbookView xWindow="732" yWindow="732" windowWidth="17280" windowHeight="8964" xr2:uid="{42AA605B-8E83-410B-8385-520117E1EEB3}"/>
   </bookViews>
   <sheets>
-    <sheet name="takvim" sheetId="2" r:id="rId1"/>
+    <sheet name="turkiyegazetesi" sheetId="3" r:id="rId1"/>
+    <sheet name="takvim" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1845" uniqueCount="1407">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1868" uniqueCount="1419">
   <si>
     <t>Account Tag</t>
   </si>
@@ -4427,6 +4428,45 @@
   </si>
   <si>
     <t>https://twitter.com/takvim/status/1739157040541422014</t>
+  </si>
+  <si>
+    <t>Screenshot Path</t>
+  </si>
+  <si>
+    <t>turkiyegazetesi</t>
+  </si>
+  <si>
+    <t>ÖÖ 12:58 · 9 May 2024</t>
+  </si>
+  <si>
+    <t>1.079 Görüntülenme</t>
+  </si>
+  <si>
+    <t>#SONDAKİKA — Akdeniz'de 3,8 büyüklüğünde deprem oldu. Deprem başta Muğla olmak üzere 5 ili etkiledi. 
+AFAD ve Kandilli, depreme ilişkin verileri açıkladı.</t>
+  </si>
+  <si>
+    <t>https://twitter.com/turkiyegazetesi/status/1788327750014537904</t>
+  </si>
+  <si>
+    <t>TweetScreenshots\2024-05-09\turkiyegazetesi\0.jpg</t>
+  </si>
+  <si>
+    <t>ÖÖ 12:42 · 9 May 2024</t>
+  </si>
+  <si>
+    <t>869 Görüntülenme</t>
+  </si>
+  <si>
+    <t>İBB, su birikintisine düşerek ölen  Eda Nur Gezer'in ölümüne ilişkin tahkikatı tamamladı:
+•  Kusuru tespit edilen 4 kişinin ihracını istendi
+• Ağaç AŞ personelinin, İBB Park ve Bahçeler Dairesi Başkanlığına bilgi vermeden işlem yaptığı tespit edildi</t>
+  </si>
+  <si>
+    <t>https://twitter.com/turkiyegazetesi/status/1788323726800355653</t>
+  </si>
+  <si>
+    <t>TweetScreenshots\2024-05-09\turkiyegazetesi\1.jpg</t>
   </si>
 </sst>
 </file>
@@ -4782,16 +4822,134 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12A2B90B-FD65-4724-B6B4-8B0BF96C83D9}">
+  <dimension ref="A1:K3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>1407</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="302.39999999999998" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1408</v>
+      </c>
+      <c r="B2" s="1">
+        <v>45421</v>
+      </c>
+      <c r="C2" s="1">
+        <v>45417</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1409</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1410</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>3</v>
+      </c>
+      <c r="H2">
+        <v>6</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>1411</v>
+      </c>
+      <c r="J2" t="s">
+        <v>1412</v>
+      </c>
+      <c r="K2" t="s">
+        <v>1413</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>1408</v>
+      </c>
+      <c r="B3" s="1">
+        <v>45421</v>
+      </c>
+      <c r="C3" s="1">
+        <v>45417</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1414</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1415</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>3</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>1416</v>
+      </c>
+      <c r="J3" t="s">
+        <v>1417</v>
+      </c>
+      <c r="K3" t="s">
+        <v>1418</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7059F1CE-17D1-4F06-95E6-631F02A8B8D3}">
   <dimension ref="A1:J368"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A292" workbookViewId="0">
+    <sheetView topLeftCell="A292" workbookViewId="0">
       <selection activeCell="H7" sqref="A1:J368"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4823,7 +4981,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -4855,7 +5013,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -4887,7 +5045,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -4919,7 +5077,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -4951,7 +5109,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -4983,7 +5141,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -5015,7 +5173,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -5047,7 +5205,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -5079,7 +5237,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -5111,7 +5269,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -5143,7 +5301,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -5175,7 +5333,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -5207,7 +5365,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -5239,7 +5397,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -5271,7 +5429,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -5303,7 +5461,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>10</v>
       </c>
@@ -5335,7 +5493,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>10</v>
       </c>
@@ -5367,7 +5525,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>10</v>
       </c>
@@ -5399,7 +5557,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -5431,7 +5589,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -5463,7 +5621,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>10</v>
       </c>
@@ -5495,7 +5653,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>10</v>
       </c>
@@ -5527,7 +5685,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>10</v>
       </c>
@@ -5559,7 +5717,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>10</v>
       </c>
@@ -5591,7 +5749,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>10</v>
       </c>
@@ -5623,7 +5781,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>10</v>
       </c>
@@ -5655,7 +5813,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>10</v>
       </c>
@@ -5687,7 +5845,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>10</v>
       </c>
@@ -5719,7 +5877,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>10</v>
       </c>
@@ -5751,7 +5909,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>10</v>
       </c>
@@ -5783,7 +5941,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>10</v>
       </c>
@@ -5815,7 +5973,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>10</v>
       </c>
@@ -5847,7 +6005,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>10</v>
       </c>
@@ -5879,7 +6037,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>10</v>
       </c>
@@ -5911,7 +6069,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>10</v>
       </c>
@@ -5943,7 +6101,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>10</v>
       </c>
@@ -5975,7 +6133,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>10</v>
       </c>
@@ -6007,7 +6165,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>10</v>
       </c>
@@ -6039,7 +6197,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>10</v>
       </c>
@@ -6071,7 +6229,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>10</v>
       </c>
@@ -6103,7 +6261,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>10</v>
       </c>
@@ -6135,7 +6293,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>10</v>
       </c>
@@ -6167,7 +6325,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>10</v>
       </c>
@@ -6199,7 +6357,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>10</v>
       </c>
@@ -6231,7 +6389,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>10</v>
       </c>
@@ -6263,7 +6421,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>10</v>
       </c>
@@ -6295,7 +6453,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>10</v>
       </c>
@@ -6327,7 +6485,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="49" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>10</v>
       </c>
@@ -6359,7 +6517,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="50" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>10</v>
       </c>
@@ -6391,7 +6549,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="51" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>10</v>
       </c>
@@ -6423,7 +6581,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="52" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>10</v>
       </c>
@@ -6455,7 +6613,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>10</v>
       </c>
@@ -6487,7 +6645,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="54" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>10</v>
       </c>
@@ -6519,7 +6677,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="55" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>10</v>
       </c>
@@ -6551,7 +6709,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="56" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>10</v>
       </c>
@@ -6583,7 +6741,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="57" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>10</v>
       </c>
@@ -6615,7 +6773,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="58" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>10</v>
       </c>
@@ -6647,7 +6805,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="59" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>10</v>
       </c>
@@ -6679,7 +6837,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="60" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>10</v>
       </c>
@@ -6711,7 +6869,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="61" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>10</v>
       </c>
@@ -6743,7 +6901,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="62" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>10</v>
       </c>
@@ -6775,7 +6933,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="63" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>10</v>
       </c>
@@ -6807,7 +6965,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="64" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>10</v>
       </c>
@@ -6839,7 +6997,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="65" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>10</v>
       </c>
@@ -6871,7 +7029,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="66" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>10</v>
       </c>
@@ -6903,7 +7061,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="67" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>10</v>
       </c>
@@ -6935,7 +7093,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="68" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>10</v>
       </c>
@@ -6967,7 +7125,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="69" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>10</v>
       </c>
@@ -6999,7 +7157,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="70" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>10</v>
       </c>
@@ -7031,7 +7189,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="71" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>10</v>
       </c>
@@ -7063,7 +7221,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="72" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>10</v>
       </c>
@@ -7095,7 +7253,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="73" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>10</v>
       </c>
@@ -7127,7 +7285,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="74" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>10</v>
       </c>
@@ -7159,7 +7317,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="75" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>10</v>
       </c>
@@ -7191,7 +7349,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="76" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>10</v>
       </c>
@@ -7223,7 +7381,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="77" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>10</v>
       </c>
@@ -7255,7 +7413,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="78" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>10</v>
       </c>
@@ -7287,7 +7445,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="79" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>10</v>
       </c>
@@ -7319,7 +7477,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="80" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>10</v>
       </c>
@@ -7351,7 +7509,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="81" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>10</v>
       </c>
@@ -7383,7 +7541,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="82" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>10</v>
       </c>
@@ -7415,7 +7573,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="83" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>10</v>
       </c>
@@ -7447,7 +7605,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="84" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>10</v>
       </c>
@@ -7479,7 +7637,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="85" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>10</v>
       </c>
@@ -7511,7 +7669,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="86" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>10</v>
       </c>
@@ -7543,7 +7701,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="87" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>10</v>
       </c>
@@ -7575,7 +7733,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="88" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>10</v>
       </c>
@@ -7607,7 +7765,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="89" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>10</v>
       </c>
@@ -7639,7 +7797,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="90" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>10</v>
       </c>
@@ -7671,7 +7829,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="91" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>10</v>
       </c>
@@ -7703,7 +7861,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="92" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>10</v>
       </c>
@@ -7735,7 +7893,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="93" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>10</v>
       </c>
@@ -7767,7 +7925,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="94" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>10</v>
       </c>
@@ -7799,7 +7957,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="95" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>10</v>
       </c>
@@ -7831,7 +7989,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="96" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>10</v>
       </c>
@@ -7863,7 +8021,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="97" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>10</v>
       </c>
@@ -7895,7 +8053,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="98" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>10</v>
       </c>
@@ -7927,7 +8085,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="99" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>10</v>
       </c>
@@ -7959,7 +8117,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="100" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>10</v>
       </c>
@@ -7991,7 +8149,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="101" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>10</v>
       </c>
@@ -8023,7 +8181,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="102" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>10</v>
       </c>
@@ -8055,7 +8213,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="103" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>10</v>
       </c>
@@ -8087,7 +8245,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="104" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>10</v>
       </c>
@@ -8119,7 +8277,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="105" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>10</v>
       </c>
@@ -8151,7 +8309,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="106" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>10</v>
       </c>
@@ -8183,7 +8341,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="107" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>10</v>
       </c>
@@ -8215,7 +8373,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="108" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>10</v>
       </c>
@@ -8247,7 +8405,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="109" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>10</v>
       </c>
@@ -8279,7 +8437,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="110" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>10</v>
       </c>
@@ -8311,7 +8469,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="111" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>10</v>
       </c>
@@ -8343,7 +8501,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="112" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>10</v>
       </c>
@@ -8375,7 +8533,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="113" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>10</v>
       </c>
@@ -8407,7 +8565,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="114" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>10</v>
       </c>
@@ -8439,7 +8597,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="115" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>10</v>
       </c>
@@ -8471,7 +8629,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="116" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>10</v>
       </c>
@@ -8503,7 +8661,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="117" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>10</v>
       </c>
@@ -8535,7 +8693,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="118" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>10</v>
       </c>
@@ -8567,7 +8725,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="119" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>10</v>
       </c>
@@ -8599,7 +8757,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="120" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>10</v>
       </c>
@@ -8631,7 +8789,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="121" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>10</v>
       </c>
@@ -8663,7 +8821,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="122" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>10</v>
       </c>
@@ -8695,7 +8853,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="123" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>10</v>
       </c>
@@ -8727,7 +8885,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="124" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>10</v>
       </c>
@@ -8759,7 +8917,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="125" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>10</v>
       </c>
@@ -8791,7 +8949,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="126" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>10</v>
       </c>
@@ -8823,7 +8981,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="127" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>10</v>
       </c>
@@ -8855,7 +9013,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="128" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>10</v>
       </c>
@@ -8887,7 +9045,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="129" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>10</v>
       </c>
@@ -8919,7 +9077,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="130" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>10</v>
       </c>
@@ -8951,7 +9109,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="131" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>10</v>
       </c>
@@ -8983,7 +9141,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="132" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>10</v>
       </c>
@@ -9015,7 +9173,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="133" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>10</v>
       </c>
@@ -9047,7 +9205,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="134" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>10</v>
       </c>
@@ -9079,7 +9237,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="135" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>10</v>
       </c>
@@ -9111,7 +9269,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="136" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>10</v>
       </c>
@@ -9143,7 +9301,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="137" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>10</v>
       </c>
@@ -9175,7 +9333,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="138" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>10</v>
       </c>
@@ -9207,7 +9365,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="139" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>10</v>
       </c>
@@ -9239,7 +9397,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="140" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>10</v>
       </c>
@@ -9271,7 +9429,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="141" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>10</v>
       </c>
@@ -9303,7 +9461,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="142" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>10</v>
       </c>
@@ -9335,7 +9493,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="143" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>10</v>
       </c>
@@ -9367,7 +9525,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="144" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>10</v>
       </c>
@@ -9399,7 +9557,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="145" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>10</v>
       </c>
@@ -9431,7 +9589,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="146" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>10</v>
       </c>
@@ -9463,7 +9621,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="147" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>10</v>
       </c>
@@ -9495,7 +9653,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="148" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>10</v>
       </c>
@@ -9527,7 +9685,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="149" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>10</v>
       </c>
@@ -9559,7 +9717,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="150" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>10</v>
       </c>
@@ -9591,7 +9749,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="151" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>10</v>
       </c>
@@ -9623,7 +9781,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="152" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>10</v>
       </c>
@@ -9655,7 +9813,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="153" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>10</v>
       </c>
@@ -9687,7 +9845,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="154" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>10</v>
       </c>
@@ -9719,7 +9877,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="155" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>10</v>
       </c>
@@ -9751,7 +9909,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="156" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>10</v>
       </c>
@@ -9783,7 +9941,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="157" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>10</v>
       </c>
@@ -9815,7 +9973,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="158" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>10</v>
       </c>
@@ -9847,7 +10005,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="159" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>10</v>
       </c>
@@ -9879,7 +10037,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="160" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>10</v>
       </c>
@@ -9911,7 +10069,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="161" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>10</v>
       </c>
@@ -9943,7 +10101,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="162" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>10</v>
       </c>
@@ -9975,7 +10133,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="163" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>10</v>
       </c>
@@ -10007,7 +10165,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="164" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>10</v>
       </c>
@@ -10039,7 +10197,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="165" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>10</v>
       </c>
@@ -10071,7 +10229,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="166" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>10</v>
       </c>
@@ -10103,7 +10261,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="167" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>10</v>
       </c>
@@ -10135,7 +10293,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="168" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>10</v>
       </c>
@@ -10167,7 +10325,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="169" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>10</v>
       </c>
@@ -10199,7 +10357,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="170" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>10</v>
       </c>
@@ -10231,7 +10389,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="171" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>10</v>
       </c>
@@ -10263,7 +10421,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="172" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>10</v>
       </c>
@@ -10295,7 +10453,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="173" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>10</v>
       </c>
@@ -10327,7 +10485,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="174" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>10</v>
       </c>
@@ -10359,7 +10517,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="175" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>10</v>
       </c>
@@ -10391,7 +10549,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="176" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>10</v>
       </c>
@@ -10423,7 +10581,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="177" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>10</v>
       </c>
@@ -10455,7 +10613,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="178" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>10</v>
       </c>
@@ -10487,7 +10645,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="179" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>10</v>
       </c>
@@ -10519,7 +10677,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="180" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>10</v>
       </c>
@@ -10551,7 +10709,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="181" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>10</v>
       </c>
@@ -10583,7 +10741,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="182" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>10</v>
       </c>
@@ -10615,7 +10773,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="183" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>10</v>
       </c>
@@ -10647,7 +10805,7 @@
         <v>715</v>
       </c>
     </row>
-    <row r="184" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>10</v>
       </c>
@@ -10679,7 +10837,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="185" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>10</v>
       </c>
@@ -10711,7 +10869,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="186" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>10</v>
       </c>
@@ -10743,7 +10901,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="187" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>10</v>
       </c>
@@ -10775,7 +10933,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="188" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>10</v>
       </c>
@@ -10807,7 +10965,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="189" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>10</v>
       </c>
@@ -10839,7 +10997,7 @@
         <v>739</v>
       </c>
     </row>
-    <row r="190" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>10</v>
       </c>
@@ -10871,7 +11029,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="191" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>10</v>
       </c>
@@ -10903,7 +11061,7 @@
         <v>747</v>
       </c>
     </row>
-    <row r="192" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>10</v>
       </c>
@@ -10935,7 +11093,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="193" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>10</v>
       </c>
@@ -10967,7 +11125,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="194" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>10</v>
       </c>
@@ -10999,7 +11157,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="195" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>10</v>
       </c>
@@ -11031,7 +11189,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="196" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>10</v>
       </c>
@@ -11063,7 +11221,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="197" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>10</v>
       </c>
@@ -11095,7 +11253,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="198" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>10</v>
       </c>
@@ -11127,7 +11285,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="199" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>10</v>
       </c>
@@ -11159,7 +11317,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="200" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>10</v>
       </c>
@@ -11191,7 +11349,7 @@
         <v>781</v>
       </c>
     </row>
-    <row r="201" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>10</v>
       </c>
@@ -11223,7 +11381,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="202" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>10</v>
       </c>
@@ -11255,7 +11413,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="203" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>10</v>
       </c>
@@ -11287,7 +11445,7 @@
         <v>793</v>
       </c>
     </row>
-    <row r="204" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>10</v>
       </c>
@@ -11319,7 +11477,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="205" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>10</v>
       </c>
@@ -11351,7 +11509,7 @@
         <v>801</v>
       </c>
     </row>
-    <row r="206" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>10</v>
       </c>
@@ -11383,7 +11541,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="207" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>10</v>
       </c>
@@ -11415,7 +11573,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="208" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
         <v>10</v>
       </c>
@@ -11447,7 +11605,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="209" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>10</v>
       </c>
@@ -11479,7 +11637,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="210" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
         <v>10</v>
       </c>
@@ -11511,7 +11669,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="211" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
         <v>10</v>
       </c>
@@ -11543,7 +11701,7 @@
         <v>824</v>
       </c>
     </row>
-    <row r="212" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
         <v>10</v>
       </c>
@@ -11575,7 +11733,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="213" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
         <v>10</v>
       </c>
@@ -11607,7 +11765,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="214" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
         <v>10</v>
       </c>
@@ -11639,7 +11797,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="215" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
         <v>10</v>
       </c>
@@ -11671,7 +11829,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="216" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
         <v>10</v>
       </c>
@@ -11703,7 +11861,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="217" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
         <v>10</v>
       </c>
@@ -11735,7 +11893,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="218" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
         <v>10</v>
       </c>
@@ -11767,7 +11925,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="219" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
         <v>10</v>
       </c>
@@ -11799,7 +11957,7 @@
         <v>854</v>
       </c>
     </row>
-    <row r="220" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
         <v>10</v>
       </c>
@@ -11831,7 +11989,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="221" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
         <v>10</v>
       </c>
@@ -11863,7 +12021,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="222" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
         <v>10</v>
       </c>
@@ -11895,7 +12053,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="223" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
         <v>10</v>
       </c>
@@ -11927,7 +12085,7 @@
         <v>870</v>
       </c>
     </row>
-    <row r="224" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
         <v>10</v>
       </c>
@@ -11959,7 +12117,7 @@
         <v>874</v>
       </c>
     </row>
-    <row r="225" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
         <v>10</v>
       </c>
@@ -11991,7 +12149,7 @@
         <v>877</v>
       </c>
     </row>
-    <row r="226" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
         <v>10</v>
       </c>
@@ -12023,7 +12181,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="227" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
         <v>10</v>
       </c>
@@ -12055,7 +12213,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="228" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
         <v>10</v>
       </c>
@@ -12087,7 +12245,7 @@
         <v>889</v>
       </c>
     </row>
-    <row r="229" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
         <v>10</v>
       </c>
@@ -12119,7 +12277,7 @@
         <v>893</v>
       </c>
     </row>
-    <row r="230" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
         <v>10</v>
       </c>
@@ -12151,7 +12309,7 @@
         <v>897</v>
       </c>
     </row>
-    <row r="231" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
         <v>10</v>
       </c>
@@ -12183,7 +12341,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="232" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
         <v>10</v>
       </c>
@@ -12215,7 +12373,7 @@
         <v>904</v>
       </c>
     </row>
-    <row r="233" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
         <v>10</v>
       </c>
@@ -12247,7 +12405,7 @@
         <v>908</v>
       </c>
     </row>
-    <row r="234" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
         <v>10</v>
       </c>
@@ -12279,7 +12437,7 @@
         <v>912</v>
       </c>
     </row>
-    <row r="235" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
         <v>10</v>
       </c>
@@ -12311,7 +12469,7 @@
         <v>915</v>
       </c>
     </row>
-    <row r="236" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
         <v>10</v>
       </c>
@@ -12343,7 +12501,7 @@
         <v>918</v>
       </c>
     </row>
-    <row r="237" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
         <v>10</v>
       </c>
@@ -12375,7 +12533,7 @@
         <v>922</v>
       </c>
     </row>
-    <row r="238" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
         <v>10</v>
       </c>
@@ -12407,7 +12565,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="239" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
         <v>10</v>
       </c>
@@ -12439,7 +12597,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="240" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
         <v>10</v>
       </c>
@@ -12471,7 +12629,7 @@
         <v>933</v>
       </c>
     </row>
-    <row r="241" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
         <v>10</v>
       </c>
@@ -12503,7 +12661,7 @@
         <v>936</v>
       </c>
     </row>
-    <row r="242" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
         <v>10</v>
       </c>
@@ -12535,7 +12693,7 @@
         <v>940</v>
       </c>
     </row>
-    <row r="243" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
         <v>10</v>
       </c>
@@ -12567,7 +12725,7 @@
         <v>944</v>
       </c>
     </row>
-    <row r="244" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
         <v>10</v>
       </c>
@@ -12599,7 +12757,7 @@
         <v>948</v>
       </c>
     </row>
-    <row r="245" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
         <v>10</v>
       </c>
@@ -12631,7 +12789,7 @@
         <v>952</v>
       </c>
     </row>
-    <row r="246" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
         <v>10</v>
       </c>
@@ -12663,7 +12821,7 @@
         <v>956</v>
       </c>
     </row>
-    <row r="247" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
         <v>10</v>
       </c>
@@ -12695,7 +12853,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="248" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
         <v>10</v>
       </c>
@@ -12727,7 +12885,7 @@
         <v>963</v>
       </c>
     </row>
-    <row r="249" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
         <v>10</v>
       </c>
@@ -12759,7 +12917,7 @@
         <v>967</v>
       </c>
     </row>
-    <row r="250" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
         <v>10</v>
       </c>
@@ -12791,7 +12949,7 @@
         <v>970</v>
       </c>
     </row>
-    <row r="251" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
         <v>10</v>
       </c>
@@ -12823,7 +12981,7 @@
         <v>973</v>
       </c>
     </row>
-    <row r="252" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
         <v>10</v>
       </c>
@@ -12855,7 +13013,7 @@
         <v>976</v>
       </c>
     </row>
-    <row r="253" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
         <v>10</v>
       </c>
@@ -12887,7 +13045,7 @@
         <v>980</v>
       </c>
     </row>
-    <row r="254" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
         <v>10</v>
       </c>
@@ -12919,7 +13077,7 @@
         <v>984</v>
       </c>
     </row>
-    <row r="255" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
         <v>10</v>
       </c>
@@ -12951,7 +13109,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="256" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
         <v>10</v>
       </c>
@@ -12983,7 +13141,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="257" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
         <v>10</v>
       </c>
@@ -13015,7 +13173,7 @@
         <v>996</v>
       </c>
     </row>
-    <row r="258" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
         <v>10</v>
       </c>
@@ -13047,7 +13205,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="259" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
         <v>10</v>
       </c>
@@ -13079,7 +13237,7 @@
         <v>1004</v>
       </c>
     </row>
-    <row r="260" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
         <v>10</v>
       </c>
@@ -13111,7 +13269,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="261" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
         <v>10</v>
       </c>
@@ -13143,7 +13301,7 @@
         <v>1011</v>
       </c>
     </row>
-    <row r="262" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
         <v>10</v>
       </c>
@@ -13175,7 +13333,7 @@
         <v>1015</v>
       </c>
     </row>
-    <row r="263" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
         <v>10</v>
       </c>
@@ -13207,7 +13365,7 @@
         <v>1018</v>
       </c>
     </row>
-    <row r="264" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
         <v>10</v>
       </c>
@@ -13239,7 +13397,7 @@
         <v>1022</v>
       </c>
     </row>
-    <row r="265" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
         <v>10</v>
       </c>
@@ -13271,7 +13429,7 @@
         <v>1026</v>
       </c>
     </row>
-    <row r="266" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
         <v>10</v>
       </c>
@@ -13303,7 +13461,7 @@
         <v>1030</v>
       </c>
     </row>
-    <row r="267" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
         <v>10</v>
       </c>
@@ -13335,7 +13493,7 @@
         <v>1034</v>
       </c>
     </row>
-    <row r="268" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
         <v>10</v>
       </c>
@@ -13367,7 +13525,7 @@
         <v>1038</v>
       </c>
     </row>
-    <row r="269" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
         <v>10</v>
       </c>
@@ -13399,7 +13557,7 @@
         <v>1042</v>
       </c>
     </row>
-    <row r="270" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
         <v>10</v>
       </c>
@@ -13431,7 +13589,7 @@
         <v>1046</v>
       </c>
     </row>
-    <row r="271" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
         <v>10</v>
       </c>
@@ -13463,7 +13621,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="272" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
         <v>10</v>
       </c>
@@ -13495,7 +13653,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="273" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
         <v>10</v>
       </c>
@@ -13527,7 +13685,7 @@
         <v>1058</v>
       </c>
     </row>
-    <row r="274" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
         <v>10</v>
       </c>
@@ -13559,7 +13717,7 @@
         <v>1062</v>
       </c>
     </row>
-    <row r="275" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
         <v>10</v>
       </c>
@@ -13591,7 +13749,7 @@
         <v>1066</v>
       </c>
     </row>
-    <row r="276" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
         <v>10</v>
       </c>
@@ -13623,7 +13781,7 @@
         <v>1070</v>
       </c>
     </row>
-    <row r="277" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
         <v>10</v>
       </c>
@@ -13655,7 +13813,7 @@
         <v>1074</v>
       </c>
     </row>
-    <row r="278" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
         <v>10</v>
       </c>
@@ -13687,7 +13845,7 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="279" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
         <v>10</v>
       </c>
@@ -13719,7 +13877,7 @@
         <v>1082</v>
       </c>
     </row>
-    <row r="280" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
         <v>10</v>
       </c>
@@ -13751,7 +13909,7 @@
         <v>1086</v>
       </c>
     </row>
-    <row r="281" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
         <v>10</v>
       </c>
@@ -13783,7 +13941,7 @@
         <v>1090</v>
       </c>
     </row>
-    <row r="282" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
         <v>10</v>
       </c>
@@ -13815,7 +13973,7 @@
         <v>1094</v>
       </c>
     </row>
-    <row r="283" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
         <v>10</v>
       </c>
@@ -13847,7 +14005,7 @@
         <v>1098</v>
       </c>
     </row>
-    <row r="284" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
         <v>10</v>
       </c>
@@ -13879,7 +14037,7 @@
         <v>1102</v>
       </c>
     </row>
-    <row r="285" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
         <v>10</v>
       </c>
@@ -13911,7 +14069,7 @@
         <v>1106</v>
       </c>
     </row>
-    <row r="286" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A286" t="s">
         <v>10</v>
       </c>
@@ -13943,7 +14101,7 @@
         <v>1109</v>
       </c>
     </row>
-    <row r="287" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
         <v>10</v>
       </c>
@@ -13975,7 +14133,7 @@
         <v>1113</v>
       </c>
     </row>
-    <row r="288" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
         <v>10</v>
       </c>
@@ -14007,7 +14165,7 @@
         <v>1116</v>
       </c>
     </row>
-    <row r="289" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
         <v>10</v>
       </c>
@@ -14039,7 +14197,7 @@
         <v>1119</v>
       </c>
     </row>
-    <row r="290" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
         <v>10</v>
       </c>
@@ -14071,7 +14229,7 @@
         <v>1123</v>
       </c>
     </row>
-    <row r="291" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
         <v>10</v>
       </c>
@@ -14103,7 +14261,7 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="292" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
         <v>10</v>
       </c>
@@ -14135,7 +14293,7 @@
         <v>1131</v>
       </c>
     </row>
-    <row r="293" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
         <v>10</v>
       </c>
@@ -14167,7 +14325,7 @@
         <v>1134</v>
       </c>
     </row>
-    <row r="294" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
         <v>10</v>
       </c>
@@ -14199,7 +14357,7 @@
         <v>1138</v>
       </c>
     </row>
-    <row r="295" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A295" t="s">
         <v>10</v>
       </c>
@@ -14231,7 +14389,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="296" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
         <v>10</v>
       </c>
@@ -14263,7 +14421,7 @@
         <v>1146</v>
       </c>
     </row>
-    <row r="297" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A297" t="s">
         <v>10</v>
       </c>
@@ -14295,7 +14453,7 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="298" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A298" t="s">
         <v>10</v>
       </c>
@@ -14327,7 +14485,7 @@
         <v>1154</v>
       </c>
     </row>
-    <row r="299" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
         <v>10</v>
       </c>
@@ -14359,7 +14517,7 @@
         <v>1158</v>
       </c>
     </row>
-    <row r="300" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A300" t="s">
         <v>10</v>
       </c>
@@ -14391,7 +14549,7 @@
         <v>1161</v>
       </c>
     </row>
-    <row r="301" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A301" t="s">
         <v>10</v>
       </c>
@@ -14423,7 +14581,7 @@
         <v>1165</v>
       </c>
     </row>
-    <row r="302" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A302" t="s">
         <v>10</v>
       </c>
@@ -14455,7 +14613,7 @@
         <v>1168</v>
       </c>
     </row>
-    <row r="303" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A303" t="s">
         <v>10</v>
       </c>
@@ -14487,7 +14645,7 @@
         <v>1171</v>
       </c>
     </row>
-    <row r="304" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A304" t="s">
         <v>10</v>
       </c>
@@ -14519,7 +14677,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="305" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A305" t="s">
         <v>10</v>
       </c>
@@ -14551,7 +14709,7 @@
         <v>1178</v>
       </c>
     </row>
-    <row r="306" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A306" t="s">
         <v>10</v>
       </c>
@@ -14583,7 +14741,7 @@
         <v>1181</v>
       </c>
     </row>
-    <row r="307" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A307" t="s">
         <v>10</v>
       </c>
@@ -14615,7 +14773,7 @@
         <v>1185</v>
       </c>
     </row>
-    <row r="308" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A308" t="s">
         <v>10</v>
       </c>
@@ -14647,7 +14805,7 @@
         <v>1188</v>
       </c>
     </row>
-    <row r="309" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A309" t="s">
         <v>10</v>
       </c>
@@ -14679,7 +14837,7 @@
         <v>1192</v>
       </c>
     </row>
-    <row r="310" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A310" t="s">
         <v>10</v>
       </c>
@@ -14711,7 +14869,7 @@
         <v>1196</v>
       </c>
     </row>
-    <row r="311" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A311" t="s">
         <v>10</v>
       </c>
@@ -14743,7 +14901,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="312" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A312" t="s">
         <v>10</v>
       </c>
@@ -14775,7 +14933,7 @@
         <v>1203</v>
       </c>
     </row>
-    <row r="313" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A313" t="s">
         <v>10</v>
       </c>
@@ -14807,7 +14965,7 @@
         <v>1207</v>
       </c>
     </row>
-    <row r="314" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A314" t="s">
         <v>10</v>
       </c>
@@ -14839,7 +14997,7 @@
         <v>1211</v>
       </c>
     </row>
-    <row r="315" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A315" t="s">
         <v>10</v>
       </c>
@@ -14871,7 +15029,7 @@
         <v>1214</v>
       </c>
     </row>
-    <row r="316" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A316" t="s">
         <v>10</v>
       </c>
@@ -14903,7 +15061,7 @@
         <v>1217</v>
       </c>
     </row>
-    <row r="317" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A317" t="s">
         <v>10</v>
       </c>
@@ -14935,7 +15093,7 @@
         <v>1221</v>
       </c>
     </row>
-    <row r="318" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A318" t="s">
         <v>10</v>
       </c>
@@ -14967,7 +15125,7 @@
         <v>1224</v>
       </c>
     </row>
-    <row r="319" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A319" t="s">
         <v>10</v>
       </c>
@@ -14999,7 +15157,7 @@
         <v>1228</v>
       </c>
     </row>
-    <row r="320" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A320" t="s">
         <v>10</v>
       </c>
@@ -15031,7 +15189,7 @@
         <v>1232</v>
       </c>
     </row>
-    <row r="321" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A321" t="s">
         <v>10</v>
       </c>
@@ -15063,7 +15221,7 @@
         <v>1236</v>
       </c>
     </row>
-    <row r="322" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A322" t="s">
         <v>10</v>
       </c>
@@ -15095,7 +15253,7 @@
         <v>1240</v>
       </c>
     </row>
-    <row r="323" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A323" t="s">
         <v>10</v>
       </c>
@@ -15127,7 +15285,7 @@
         <v>1244</v>
       </c>
     </row>
-    <row r="324" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A324" t="s">
         <v>10</v>
       </c>
@@ -15159,7 +15317,7 @@
         <v>1248</v>
       </c>
     </row>
-    <row r="325" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A325" t="s">
         <v>10</v>
       </c>
@@ -15191,7 +15349,7 @@
         <v>1251</v>
       </c>
     </row>
-    <row r="326" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A326" t="s">
         <v>10</v>
       </c>
@@ -15223,7 +15381,7 @@
         <v>1255</v>
       </c>
     </row>
-    <row r="327" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A327" t="s">
         <v>10</v>
       </c>
@@ -15255,7 +15413,7 @@
         <v>1259</v>
       </c>
     </row>
-    <row r="328" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A328" t="s">
         <v>10</v>
       </c>
@@ -15287,7 +15445,7 @@
         <v>1263</v>
       </c>
     </row>
-    <row r="329" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A329" t="s">
         <v>10</v>
       </c>
@@ -15319,7 +15477,7 @@
         <v>1267</v>
       </c>
     </row>
-    <row r="330" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A330" t="s">
         <v>10</v>
       </c>
@@ -15351,7 +15509,7 @@
         <v>1270</v>
       </c>
     </row>
-    <row r="331" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A331" t="s">
         <v>10</v>
       </c>
@@ -15383,7 +15541,7 @@
         <v>1273</v>
       </c>
     </row>
-    <row r="332" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A332" t="s">
         <v>10</v>
       </c>
@@ -15415,7 +15573,7 @@
         <v>1277</v>
       </c>
     </row>
-    <row r="333" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A333" t="s">
         <v>10</v>
       </c>
@@ -15447,7 +15605,7 @@
         <v>1281</v>
       </c>
     </row>
-    <row r="334" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A334" t="s">
         <v>10</v>
       </c>
@@ -15479,7 +15637,7 @@
         <v>1285</v>
       </c>
     </row>
-    <row r="335" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A335" t="s">
         <v>10</v>
       </c>
@@ -15511,7 +15669,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="336" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A336" t="s">
         <v>10</v>
       </c>
@@ -15543,7 +15701,7 @@
         <v>1291</v>
       </c>
     </row>
-    <row r="337" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A337" t="s">
         <v>10</v>
       </c>
@@ -15575,7 +15733,7 @@
         <v>1295</v>
       </c>
     </row>
-    <row r="338" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A338" t="s">
         <v>10</v>
       </c>
@@ -15607,7 +15765,7 @@
         <v>1299</v>
       </c>
     </row>
-    <row r="339" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A339" t="s">
         <v>10</v>
       </c>
@@ -15639,7 +15797,7 @@
         <v>1303</v>
       </c>
     </row>
-    <row r="340" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A340" t="s">
         <v>10</v>
       </c>
@@ -15671,7 +15829,7 @@
         <v>1306</v>
       </c>
     </row>
-    <row r="341" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A341" t="s">
         <v>10</v>
       </c>
@@ -15703,7 +15861,7 @@
         <v>1310</v>
       </c>
     </row>
-    <row r="342" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A342" t="s">
         <v>10</v>
       </c>
@@ -15735,7 +15893,7 @@
         <v>1314</v>
       </c>
     </row>
-    <row r="343" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A343" t="s">
         <v>10</v>
       </c>
@@ -15767,7 +15925,7 @@
         <v>1318</v>
       </c>
     </row>
-    <row r="344" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A344" t="s">
         <v>10</v>
       </c>
@@ -15799,7 +15957,7 @@
         <v>1322</v>
       </c>
     </row>
-    <row r="345" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A345" t="s">
         <v>10</v>
       </c>
@@ -15831,7 +15989,7 @@
         <v>1325</v>
       </c>
     </row>
-    <row r="346" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A346" t="s">
         <v>10</v>
       </c>
@@ -15863,7 +16021,7 @@
         <v>1328</v>
       </c>
     </row>
-    <row r="347" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A347" t="s">
         <v>10</v>
       </c>
@@ -15895,7 +16053,7 @@
         <v>1331</v>
       </c>
     </row>
-    <row r="348" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A348" t="s">
         <v>10</v>
       </c>
@@ -15927,7 +16085,7 @@
         <v>1335</v>
       </c>
     </row>
-    <row r="349" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A349" t="s">
         <v>10</v>
       </c>
@@ -15959,7 +16117,7 @@
         <v>1338</v>
       </c>
     </row>
-    <row r="350" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A350" t="s">
         <v>10</v>
       </c>
@@ -15991,7 +16149,7 @@
         <v>1341</v>
       </c>
     </row>
-    <row r="351" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A351" t="s">
         <v>10</v>
       </c>
@@ -16023,7 +16181,7 @@
         <v>1345</v>
       </c>
     </row>
-    <row r="352" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A352" t="s">
         <v>10</v>
       </c>
@@ -16055,7 +16213,7 @@
         <v>1349</v>
       </c>
     </row>
-    <row r="353" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A353" t="s">
         <v>10</v>
       </c>
@@ -16087,7 +16245,7 @@
         <v>1353</v>
       </c>
     </row>
-    <row r="354" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A354" t="s">
         <v>10</v>
       </c>
@@ -16119,7 +16277,7 @@
         <v>1356</v>
       </c>
     </row>
-    <row r="355" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A355" t="s">
         <v>10</v>
       </c>
@@ -16151,7 +16309,7 @@
         <v>1360</v>
       </c>
     </row>
-    <row r="356" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A356" t="s">
         <v>10</v>
       </c>
@@ -16183,7 +16341,7 @@
         <v>1364</v>
       </c>
     </row>
-    <row r="357" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A357" t="s">
         <v>10</v>
       </c>
@@ -16215,7 +16373,7 @@
         <v>1367</v>
       </c>
     </row>
-    <row r="358" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A358" t="s">
         <v>10</v>
       </c>
@@ -16247,7 +16405,7 @@
         <v>1371</v>
       </c>
     </row>
-    <row r="359" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A359" t="s">
         <v>10</v>
       </c>
@@ -16279,7 +16437,7 @@
         <v>1374</v>
       </c>
     </row>
-    <row r="360" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A360" t="s">
         <v>10</v>
       </c>
@@ -16311,7 +16469,7 @@
         <v>1378</v>
       </c>
     </row>
-    <row r="361" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A361" t="s">
         <v>10</v>
       </c>
@@ -16343,7 +16501,7 @@
         <v>1381</v>
       </c>
     </row>
-    <row r="362" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A362" t="s">
         <v>10</v>
       </c>
@@ -16375,7 +16533,7 @@
         <v>1385</v>
       </c>
     </row>
-    <row r="363" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A363" t="s">
         <v>10</v>
       </c>
@@ -16407,7 +16565,7 @@
         <v>1388</v>
       </c>
     </row>
-    <row r="364" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A364" t="s">
         <v>10</v>
       </c>
@@ -16439,7 +16597,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="365" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A365" t="s">
         <v>10</v>
       </c>
@@ -16471,7 +16629,7 @@
         <v>1396</v>
       </c>
     </row>
-    <row r="366" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A366" t="s">
         <v>10</v>
       </c>
@@ -16503,7 +16661,7 @@
         <v>1398</v>
       </c>
     </row>
-    <row r="367" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A367" t="s">
         <v>10</v>
       </c>
@@ -16535,7 +16693,7 @@
         <v>1402</v>
       </c>
     </row>
-    <row r="368" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A368" t="s">
         <v>10</v>
       </c>

</xml_diff>